<commit_message>
update 2020-gallery template files
</commit_message>
<xml_diff>
--- a/adcore/2020/templates/2020-gallery.xlsx
+++ b/adcore/2020/templates/2020-gallery.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/11411/Dropbox/git/repo/agency/adcore/2020/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB0810D-1308-CA44-9386-3D77C360BF31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35200824-5AA4-1D44-865A-561B09E76DE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="660" windowWidth="33200" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="895">
   <si>
     <t>Offer Code</t>
   </si>
@@ -2707,6 +2707,15 @@
   </si>
   <si>
     <t>Banner/Blank</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXX140433</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXX140533</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXX140633</t>
   </si>
 </sst>
 </file>
@@ -3131,7 +3140,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4255,7 +4266,7 @@
         <v>230</v>
       </c>
       <c r="B101" t="s">
-        <v>702</v>
+        <v>892</v>
       </c>
       <c r="C101" t="s">
         <v>231</v>
@@ -4266,7 +4277,7 @@
         <v>232</v>
       </c>
       <c r="B102" t="s">
-        <v>703</v>
+        <v>893</v>
       </c>
       <c r="C102" t="s">
         <v>233</v>
@@ -4277,7 +4288,7 @@
         <v>234</v>
       </c>
       <c r="B103" t="s">
-        <v>704</v>
+        <v>894</v>
       </c>
       <c r="C103" t="s">
         <v>235</v>

</xml_diff>